<commit_message>
Added lots of data and many summer changes
</commit_message>
<xml_diff>
--- a/Post Processing/3_4SDWritingTest/SDWritingTest3.xlsx
+++ b/Post Processing/3_4SDWritingTest/SDWritingTest3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahell\Documents\DAQ\Post Processing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahell\Documents\DAQ\Post Processing\3_4SDWritingTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7481450-F276-4964-8398-30D43832F32B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDA5410-4E1F-45A7-8FF2-1C5D8CA361AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3408" yWindow="1488" windowWidth="17280" windowHeight="9024" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -446,31 +446,12 @@
   <dimension ref="A1:BZ1067"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:BZ1"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.140625" customWidth="1"/>
-    <col min="2" max="2" width="3.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="4.140625" customWidth="1"/>
-    <col min="5" max="5" width="3.140625" customWidth="1"/>
-    <col min="6" max="6" width="2.140625" customWidth="1"/>
-    <col min="7" max="8" width="3.140625" customWidth="1"/>
-    <col min="9" max="9" width="2.140625" customWidth="1"/>
-    <col min="10" max="10" width="5.140625" customWidth="1"/>
-    <col min="11" max="11" width="4.140625" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" customWidth="1"/>
-    <col min="13" max="14" width="14.42578125" customWidth="1"/>
-    <col min="15" max="15" width="16.42578125" customWidth="1"/>
-    <col min="16" max="16" width="6.42578125" customWidth="1"/>
-    <col min="17" max="17" width="5.7109375" customWidth="1"/>
-    <col min="18" max="18" width="5.42578125" customWidth="1"/>
-    <col min="19" max="19" width="7.42578125" customWidth="1"/>
-    <col min="20" max="21" width="4.7109375" customWidth="1"/>
-    <col min="22" max="24" width="5.42578125" customWidth="1"/>
-    <col min="25" max="25" width="9.140625" customWidth="1"/>
+    <col min="1" max="25" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:78" x14ac:dyDescent="0.25">

</xml_diff>